<commit_message>
aufgeräumt, module berechnen_bs und _wp angepasst, berechnen_ev angefangen
</commit_message>
<xml_diff>
--- a/Inputs/waermebedarf.xlsx
+++ b/Inputs/waermebedarf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DianaEspinosaLozano\Desktop\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DianaEspinosaLozano\Desktop\Thesis\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB3EDF39-6FF5-4A5C-8E03-D2472EE21C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7434C314-8914-48A1-8E68-4E82CC75E816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="60" windowWidth="14610" windowHeight="15585" xr2:uid="{E1C8AC05-483C-410D-A814-D9126F8A5C87}"/>
+    <workbookView minimized="1" xWindow="-25260" yWindow="1905" windowWidth="21600" windowHeight="11100" xr2:uid="{E1C8AC05-483C-410D-A814-D9126F8A5C87}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -461,7 +461,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
wp mit und ohne hems angepasst
</commit_message>
<xml_diff>
--- a/Inputs/waermebedarf.xlsx
+++ b/Inputs/waermebedarf.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{7434C314-8914-48A1-8E68-4E82CC75E816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36AFA182-19BA-48D6-9FF3-8CF67E0B6425}"/>
   <bookViews>
-    <workbookView xWindow="-5600" yWindow="-21600" windowWidth="19380" windowHeight="20970" xr2:uid="{E1C8AC05-483C-410D-A814-D9126F8A5C87}"/>
+    <workbookView xWindow="1103" yWindow="1103" windowWidth="16200" windowHeight="9982" xr2:uid="{E1C8AC05-483C-410D-A814-D9126F8A5C87}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>